<commit_message>
Update 2020-03-17 06:35 More Carrebian and likes had to be addded
</commit_message>
<xml_diff>
--- a/COVID-19 Apps/Switzerland by Cantons.xlsx
+++ b/COVID-19 Apps/Switzerland by Cantons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zur Bonsen Georg\Documents\Programme\Beyond4P_Apps\COVID-19 Apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A6E55A-0A59-4B01-B7B2-D4B7F12F681D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2956D9-FA38-46E6-94E3-A168A7099DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{D2DEF9EE-F3E9-4F77-8BB9-00BE635697CB}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$2:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$2:$I$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>TI</t>
   </si>
@@ -119,16 +119,28 @@
     <t>Kanton</t>
   </si>
   <si>
-    <t>Fälle</t>
-  </si>
-  <si>
-    <t>Todesfälle</t>
-  </si>
-  <si>
     <t>Einwohner</t>
   </si>
   <si>
     <t>Prozent</t>
+  </si>
+  <si>
+    <t>Vgl</t>
+  </si>
+  <si>
+    <t>Fälle 15.3.</t>
+  </si>
+  <si>
+    <t>Todsf. 15.3</t>
+  </si>
+  <si>
+    <t>Fälle 16.3.</t>
+  </si>
+  <si>
+    <t>Todsf. 16.3</t>
+  </si>
+  <si>
+    <t>Delta</t>
   </si>
 </sst>
 </file>
@@ -136,9 +148,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +173,17 @@
     <font>
       <sz val="11.55"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.55"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -191,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -204,7 +227,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -286,11 +313,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$C$2</c:f>
+              <c:f>Tabelle1!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fälle</c:v>
+                  <c:v>Fälle 15.3.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -309,6 +336,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -324,6 +356,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -339,6 +376,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -354,6 +396,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -369,6 +416,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -384,6 +436,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -401,6 +458,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -418,6 +480,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -435,6 +502,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -452,6 +524,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -469,6 +546,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -510,6 +592,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -528,6 +615,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -546,6 +638,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -564,6 +661,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -582,6 +684,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -600,6 +707,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -617,6 +729,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -634,6 +751,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -651,6 +773,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -668,6 +795,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -685,6 +817,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -702,6 +839,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -720,6 +862,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -738,6 +885,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-1375-4FE1-BE39-6640E7B6D0A0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -827,7 +979,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$C$3:$C$28</c:f>
+              <c:f>Tabelle1!$D$3:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1106,7 +1258,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$F$2</c:f>
+              <c:f>Tabelle1!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1232,7 +1384,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$F$3:$F$28</c:f>
+              <c:f>Tabelle1!$I$3:$I$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="26"/>
@@ -2600,13 +2752,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>619124</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
@@ -2636,13 +2788,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>195261</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>638174</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -2970,19 +3122,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B44319F-252C-47D9-A9B6-6166235D0676}">
-  <dimension ref="B2:F28"/>
+  <dimension ref="A2:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="3" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="7"/>
+    <col min="8" max="8" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -2990,481 +3148,828 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="e">
+        <f>MATCH(B3,Q:Q,0)</f>
+        <v>#N/A</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
+        <v>353343</v>
+      </c>
+      <c r="D3" s="3">
         <v>291</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>6</v>
       </c>
-      <c r="E3" s="5">
-        <v>353343</v>
-      </c>
-      <c r="F3" s="6">
-        <f t="shared" ref="F3:F27" si="0">C3/E3</f>
+      <c r="F3" s="8">
+        <v>330</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="8">
+        <v>39</v>
+      </c>
+      <c r="I3" s="6">
+        <f>D3/C3</f>
         <v>8.2356237423693128E-4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="e">
+        <f t="shared" ref="A4:A28" si="0">MATCH(B4,Q:Q,0)</f>
+        <v>#N/A</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
+        <v>799145</v>
+      </c>
+      <c r="D4" s="3">
         <v>273</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="5">
-        <v>799145</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="F4" s="8">
+        <v>273</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <f>D4/C4</f>
+        <v>3.416151011393427E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="e">
         <f t="shared" si="0"/>
-        <v>3.416151011393427E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
+        <v>1520968</v>
+      </c>
+      <c r="D5" s="3">
         <v>148</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1520968</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>270</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8">
+        <v>122</v>
+      </c>
+      <c r="I5" s="6">
+        <f>D5/C5</f>
+        <v>9.7306452206752546E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="e">
         <f t="shared" si="0"/>
-        <v>9.7306452206752546E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
+        <v>194766</v>
+      </c>
+      <c r="D6" s="3">
         <v>119</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="5">
-        <v>194766</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="F6" s="8">
+        <v>119</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <f>D6/C6</f>
+        <v>6.1098959777373875E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="e">
         <f t="shared" si="0"/>
-        <v>6.1098959777373875E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="5">
+        <v>499480</v>
+      </c>
+      <c r="D7" s="3">
         <v>107</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="5">
-        <v>499480</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="F7" s="8">
+        <v>107</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <f>D7/C7</f>
+        <v>2.142227917033715E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="e">
         <f t="shared" si="0"/>
-        <v>2.142227917033715E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
+        <v>1034977</v>
+      </c>
+      <c r="D8" s="3">
         <v>78</v>
       </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1034977</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>104</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <v>26</v>
+      </c>
+      <c r="I8" s="6">
+        <f>D8/C8</f>
+        <v>7.5363993595992961E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="e">
         <f t="shared" si="0"/>
-        <v>7.5363993595992961E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
+        <v>288132</v>
+      </c>
+      <c r="D9" s="3">
         <v>48</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>2</v>
       </c>
-      <c r="E9" s="5">
-        <v>288132</v>
-      </c>
-      <c r="F9" s="6">
+      <c r="F9" s="8">
+        <v>48</v>
+      </c>
+      <c r="G9" s="4">
+        <v>2</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <f>D9/C9</f>
+        <v>1.6659031277331223E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="e">
         <f t="shared" si="0"/>
-        <v>1.6659031277331223E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
+        <v>198379</v>
+      </c>
+      <c r="D10" s="3">
         <v>47</v>
       </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5">
-        <v>198379</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
+        <v>47</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <f>D10/C10</f>
+        <v>2.3692023853331249E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="e">
         <f t="shared" si="0"/>
-        <v>2.3692023853331249E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
+        <v>343955</v>
+      </c>
+      <c r="D11" s="3">
         <v>47</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="5">
-        <v>343955</v>
-      </c>
-      <c r="F11" s="6">
+      <c r="F11" s="8">
+        <v>47</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <f>D11/C11</f>
+        <v>1.3664578215173497E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="e">
         <f t="shared" si="0"/>
-        <v>1.3664578215173497E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
+        <v>176850</v>
+      </c>
+      <c r="D12" s="3">
         <v>39</v>
       </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
-        <v>176850</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>39</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <f>D12/C12</f>
+        <v>2.2052586938083122E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="e">
         <f t="shared" si="0"/>
-        <v>2.2052586938083122E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
+        <v>318714</v>
+      </c>
+      <c r="D13" s="3">
         <v>38</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5">
-        <v>318714</v>
-      </c>
-      <c r="F13" s="6">
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>38</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <f>D13/C13</f>
+        <v>1.1922915215522381E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="e">
         <f t="shared" si="0"/>
-        <v>1.1922915215522381E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="5">
+        <v>677387</v>
+      </c>
+      <c r="D14" s="3">
         <v>31</v>
       </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5">
-        <v>677387</v>
-      </c>
-      <c r="F14" s="6">
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>31</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <f>D14/C14</f>
+        <v>4.5764090542038748E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="e">
         <f t="shared" si="0"/>
-        <v>4.5764090542038748E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
+        <v>507697</v>
+      </c>
+      <c r="D15" s="3">
         <v>26</v>
       </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <v>507697</v>
-      </c>
-      <c r="F15" s="6">
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>26</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <f>D15/C15</f>
+        <v>5.1211647892345237E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="e">
         <f t="shared" si="0"/>
-        <v>5.1211647892345237E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="5">
+        <v>409557</v>
+      </c>
+      <c r="D16" s="3">
         <v>19</v>
       </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5">
-        <v>409557</v>
-      </c>
-      <c r="F16" s="6">
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>26</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <v>7</v>
+      </c>
+      <c r="I16" s="6">
+        <f>D16/C16</f>
+        <v>4.6391588960755156E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="e">
         <f t="shared" si="0"/>
-        <v>4.6391588960755156E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="5">
+        <v>159165</v>
+      </c>
+      <c r="D17" s="3">
         <v>13</v>
       </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="5">
-        <v>159165</v>
-      </c>
-      <c r="F17" s="6">
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>9</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
+        <v>-4</v>
+      </c>
+      <c r="I17" s="6">
+        <f>D17/C17</f>
+        <v>8.1676247918826373E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="e">
         <f t="shared" si="0"/>
-        <v>8.1676247918826373E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
+        <v>73419</v>
+      </c>
+      <c r="D18" s="3">
         <v>10</v>
       </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5">
-        <v>73419</v>
-      </c>
-      <c r="F18" s="6">
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6">
+        <f>D18/C18</f>
+        <v>1.3620452471431102E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="e">
         <f t="shared" si="0"/>
-        <v>1.3620452471431102E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="5">
+        <v>273194</v>
+      </c>
+      <c r="D19" s="3">
         <v>10</v>
       </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
-        <v>273194</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8">
+        <v>10</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+      <c r="I19" s="6">
+        <f>D19/C19</f>
+        <v>3.6604024978586647E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="e">
         <f t="shared" si="0"/>
-        <v>3.6604024978586647E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="5">
+        <v>126837</v>
+      </c>
+      <c r="D20" s="3">
         <v>9</v>
       </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="5">
-        <v>126837</v>
-      </c>
-      <c r="F20" s="6">
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>13</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
+        <v>4</v>
+      </c>
+      <c r="I20" s="6">
+        <f>D20/C20</f>
+        <v>7.0957212800681189E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="e">
         <f t="shared" si="0"/>
-        <v>7.0957212800681189E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="5">
+        <v>37841</v>
+      </c>
+      <c r="D21" s="3">
         <v>8</v>
       </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="E21" s="5">
-        <v>37841</v>
-      </c>
-      <c r="F21" s="6">
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="8">
+        <v>-7</v>
+      </c>
+      <c r="I21" s="6">
+        <f>D21/C21</f>
+        <v>2.1141090351734892E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="e">
         <f t="shared" si="0"/>
-        <v>2.1141090351734892E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="5">
+        <v>55234</v>
+      </c>
+      <c r="D22" s="3">
         <v>5</v>
       </c>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
-      <c r="E22" s="5">
-        <v>55234</v>
-      </c>
-      <c r="F22" s="6">
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6">
+        <f>D22/C22</f>
+        <v>9.0523952637867978E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="e">
         <f t="shared" si="0"/>
-        <v>9.0523952637867978E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="5">
+        <v>43223</v>
+      </c>
+      <c r="D23" s="3">
         <v>5</v>
       </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
-        <v>43223</v>
-      </c>
-      <c r="F23" s="6">
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8">
+        <v>8</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="8">
+        <v>3</v>
+      </c>
+      <c r="I23" s="6">
+        <f>D23/C23</f>
+        <v>1.1567915230317192E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="e">
         <f t="shared" si="0"/>
-        <v>1.1567915230317192E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="5">
+        <v>276472</v>
+      </c>
+      <c r="D24" s="3">
         <v>5</v>
       </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5">
-        <v>276472</v>
-      </c>
-      <c r="F24" s="6">
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8">
+        <v>5</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6">
+        <f>D24/C24</f>
+        <v>1.8085014033970889E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="e">
         <f t="shared" si="0"/>
-        <v>1.8085014033970889E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="5">
+        <v>16145</v>
+      </c>
+      <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5">
-        <v>16145</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0</v>
+      </c>
+      <c r="I25" s="6">
+        <f>D25/C25</f>
+        <v>1.2387736141220192E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="e">
         <f t="shared" si="0"/>
-        <v>1.2387736141220192E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="5">
+        <v>40403</v>
+      </c>
+      <c r="D26" s="3">
         <v>2</v>
       </c>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5">
-        <v>40403</v>
-      </c>
-      <c r="F26" s="6">
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="8">
+        <v>2</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="8">
+        <v>0</v>
+      </c>
+      <c r="I26" s="6">
+        <f>D26/C26</f>
+        <v>4.9501274657822438E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="e">
         <f t="shared" si="0"/>
-        <v>4.9501274657822438E-5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="5">
+        <v>81991</v>
+      </c>
+      <c r="D27" s="3">
         <v>1</v>
       </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5">
-        <v>81991</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0</v>
+      </c>
+      <c r="I27" s="6">
+        <f>D27/C27</f>
+        <v>1.2196460587137613E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="e">
         <f t="shared" si="0"/>
-        <v>1.2196460587137613E-5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>#N/A</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="5">
+        <v>36433</v>
+      </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="5">
-        <v>36433</v>
-      </c>
-      <c r="F28" s="6">
-        <f>C28/E28</f>
+      <c r="E28" s="1"/>
+      <c r="F28" s="8">
+        <v>2</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="8">
+        <v>2</v>
+      </c>
+      <c r="I28" s="6">
+        <f>D28/C28</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:F2" xr:uid="{C199DFAA-92C5-40AD-BC17-72F2093E82FF}"/>
+  <autoFilter ref="B2:I2" xr:uid="{C199DFAA-92C5-40AD-BC17-72F2093E82FF}"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>